<commit_message>
tbh I don't 100% remember what I changed, but xlsx isn't the best format for version control anyways.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fynn/Desktop/projekte/bachelor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18173BBF-15AF-3E40-98CB-6239988BFD53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F547360F-4E61-C045-B21A-791B814C5A53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="480" windowWidth="33600" windowHeight="20540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta data" sheetId="1" r:id="rId1"/>
@@ -33,8 +33,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4005" uniqueCount="1353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4010" uniqueCount="1357">
   <si>
     <t>DEFINITIONS</t>
   </si>
@@ -4093,14 +4115,34 @@
   </si>
   <si>
     <t>Der allgemeine Stundenweltrekord für ausschließlich mit eigener Muskelkraft betriebene Fahrzeuge liegt deutlich über dem Rekord mit einem klassischen Rennrad. Die Französin Barbara Buatois fuhr mit einem vollverkleideten Liegerad am 19. Juli 2009 im US-amerikanischen Romeo eine Strecke von 84,02 km, womit sie als erste Frau eine Strecke von mehr als 80 km in einer Stunde mit einem Liegerad zurücklegte. Den aktuellen Stundenweltrekord der Männer hält der Schweizer Francesco Russo; er fuhr am 26. Juni 2016 im deutschen Klettwitz 92,43 km.</t>
+  </si>
+  <si>
+    <t>after selection</t>
+  </si>
+  <si>
+    <t># paragraphs</t>
+  </si>
+  <si>
+    <t># articles</t>
+  </si>
+  <si>
+    <t>avg # sentences</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -4128,8 +4170,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4698,10 +4741,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B8:N19"/>
+  <dimension ref="B8:N29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4739,7 +4782,7 @@
         <v>1348</v>
       </c>
     </row>
-    <row r="17" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:14" x14ac:dyDescent="0.2">
       <c r="M17" t="s">
         <v>1349</v>
       </c>
@@ -4748,7 +4791,7 @@
         <v>105.15884773662552</v>
       </c>
     </row>
-    <row r="18" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:14" x14ac:dyDescent="0.2">
       <c r="M18" t="s">
         <v>1350</v>
       </c>
@@ -4757,13 +4800,54 @@
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:14" x14ac:dyDescent="0.2">
       <c r="M19" t="s">
         <v>1351</v>
       </c>
       <c r="N19">
         <f t="array" ref="N19">SUMPRODUCT(--(all_paragraphs!F2:F1216 = all_paragraphs!G2:G1216),all_paragraphs!G2:G1216, all_paragraphs!H2:H1216) / N18</f>
         <v>102.09565217391304</v>
+      </c>
+    </row>
+    <row r="25" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D25" s="1" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="26" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D26">
+        <f>COUNT(paragraphs!A:A)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D27" cm="1">
+        <f t="array" ref="D27">SUM(1/COUNTIF(paragraphs!D2:D61, paragraphs!D2:D61))</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>1349</v>
+      </c>
+      <c r="D28">
+        <f>SUMPRODUCT(paragraphs!F:F, paragraphs!H:H)/D26</f>
+        <v>100.5</v>
+      </c>
+    </row>
+    <row r="29" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>1356</v>
+      </c>
+      <c r="D29">
+        <f>AVERAGE(paragraphs!F:F)</f>
+        <v>4.8666666666666663</v>
       </c>
     </row>
   </sheetData>
@@ -52166,8 +52250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>